<commit_message>
Arreglo de respuesta de funciones a JsonResponse
</commit_message>
<xml_diff>
--- a/temp_files/estudiantes_invalidos.xlsx
+++ b/temp_files/estudiantes_invalidos.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -647,17 +647,21 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1725526800</v>
+        <v>1725958800</v>
       </c>
       <c r="G2" t="n">
-        <v>1727686800</v>
+        <v>1728118800</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>SIN MOVIL</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
+          <t>3209006290</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>573209006290</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>LA CALERA</t>
@@ -808,10 +812,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1725526800</v>
+        <v>1725958800</v>
       </c>
       <c r="G3" t="n">
-        <v>1725526800</v>
+        <v>1725958800</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -969,10 +973,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1725526800</v>
+        <v>1725958800</v>
       </c>
       <c r="G4" t="n">
-        <v>1726131600</v>
+        <v>1726563600</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
HOTFIX `core_users_update_users.py`cambios para verificar el error de userid en core users update users
</commit_message>
<xml_diff>
--- a/temp_files/estudiantes_invalidos.xlsx
+++ b/temp_files/estudiantes_invalidos.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -647,21 +647,17 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1725958800</v>
+        <v>1725526800</v>
       </c>
       <c r="G2" t="n">
-        <v>1728118800</v>
+        <v>1727686800</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>3209006290</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>573209006290</t>
-        </is>
-      </c>
+          <t>SIN MOVIL</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
           <t>LA CALERA</t>
@@ -781,7 +777,7 @@
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>NO está en la BD esa cédula</t>
+          <t>Existe en la BD</t>
         </is>
       </c>
     </row>
@@ -812,10 +808,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1725958800</v>
+        <v>1725526800</v>
       </c>
       <c r="G3" t="n">
-        <v>1725958800</v>
+        <v>1725526800</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -942,7 +938,7 @@
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>NO está en la BD esa cédula</t>
+          <t>Existe en la BD</t>
         </is>
       </c>
     </row>
@@ -973,10 +969,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1725958800</v>
+        <v>1725526800</v>
       </c>
       <c r="G4" t="n">
-        <v>1726563600</v>
+        <v>1726131600</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1109,7 +1105,7 @@
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>NO está en la BD esa cédula</t>
+          <t>Existe en la BD</t>
         </is>
       </c>
     </row>

</xml_diff>